<commit_message>
any more spelling mistakes are not my business
</commit_message>
<xml_diff>
--- a/data/TendaguruNames.xlsx
+++ b/data/TendaguruNames.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicit\OneDrive\Dokumente\Master\2ndSemester\ResearchProject\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicit\OneDrive\Dokumente\Master\2ndSemester\ResearchProject\Research_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A455994E-F072-4688-9048-F33968552695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA330516-F1A6-43D0-9C05-D4A5D6790E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,9 +256,6 @@
     <t>1990: original brachiosaurus bones were agreed to be loaned to "a Dutch museum"</t>
   </si>
   <si>
-    <t>brancia</t>
-  </si>
-  <si>
     <t>Wilhelm von Branca (director of Museum für Naturkunde)</t>
   </si>
   <si>
@@ -586,9 +583,6 @@
     <t>"largest"</t>
   </si>
   <si>
-    <t>androdemus</t>
-  </si>
-  <si>
     <t>antrodemus tendagurensis</t>
   </si>
   <si>
@@ -647,6 +641,12 @@
   </si>
   <si>
     <t>scientist</t>
+  </si>
+  <si>
+    <t>brancai</t>
+  </si>
+  <si>
+    <t>antrodemus</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -725,7 +725,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -943,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -988,7 +987,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1058,7 +1057,7 @@
         <v>23</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I3" s="3">
         <v>1894</v>
@@ -1117,7 +1116,7 @@
         <v>32</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I4" s="3">
         <v>1919</v>
@@ -1167,7 +1166,7 @@
         <v>39</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I5" s="3">
         <v>1919</v>
@@ -1217,7 +1216,7 @@
         <v>44</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I6" s="3">
         <v>1915</v>
@@ -1267,7 +1266,7 @@
         <v>49</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I7" s="3">
         <v>1915</v>
@@ -1320,7 +1319,7 @@
         <v>55</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I9" s="3">
         <v>1865</v>
@@ -1379,7 +1378,7 @@
         <v>59</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I10" s="3">
         <v>2007</v>
@@ -1426,7 +1425,7 @@
         <v>64</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I11" s="3">
         <v>2007</v>
@@ -1473,7 +1472,7 @@
         <v>68</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I12" s="3">
         <v>1890</v>
@@ -1523,7 +1522,7 @@
         <v>71</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I13" s="3">
         <v>1908</v>
@@ -1541,7 +1540,7 @@
         <v>25</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>28</v>
@@ -1570,7 +1569,7 @@
         <v>75</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I14" s="3">
         <v>1903</v>
@@ -1608,7 +1607,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>78</v>
+        <v>207</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
@@ -1620,16 +1619,16 @@
         <v>38</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I15" s="3">
         <v>1914</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>25</v>
@@ -1655,10 +1654,10 @@
         <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>37</v>
@@ -1670,16 +1669,16 @@
         <v>38</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I16" s="3">
         <v>1914</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>25</v>
@@ -1714,10 +1713,10 @@
         <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>20</v>
@@ -1729,16 +1728,16 @@
         <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I17" s="3">
         <v>1914</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>25</v>
@@ -1764,10 +1763,10 @@
         <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>37</v>
@@ -1779,16 +1778,16 @@
         <v>38</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I18" s="3">
         <v>1914</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>25</v>
@@ -1814,10 +1813,10 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>37</v>
@@ -1829,16 +1828,16 @@
         <v>38</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I19" s="3">
         <v>1914</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>25</v>
@@ -1861,10 +1860,10 @@
         <v>51</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>20</v>
@@ -1876,22 +1875,22 @@
         <v>22</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I20" s="3">
         <v>1869</v>
       </c>
       <c r="J20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>25</v>
@@ -1908,10 +1907,10 @@
         <v>51</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>37</v>
@@ -1923,10 +1922,10 @@
         <v>22</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I21" s="3">
         <v>1908</v>
@@ -1944,7 +1943,7 @@
         <v>25</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>28</v>
@@ -1955,10 +1954,10 @@
         <v>51</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>20</v>
@@ -1970,16 +1969,16 @@
         <v>22</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I22" s="3">
         <v>1988</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>25</v>
@@ -1991,7 +1990,7 @@
         <v>25</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O22" s="2" t="s">
         <v>28</v>
@@ -2002,10 +2001,10 @@
         <v>51</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>20</v>
@@ -2017,16 +2016,16 @@
         <v>38</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I23" s="3">
         <v>1991</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>25</v>
@@ -2049,10 +2048,10 @@
         <v>51</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>20</v>
@@ -2064,22 +2063,22 @@
         <v>48</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I24" s="3">
         <v>2000</v>
       </c>
       <c r="J24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="K24" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="L24" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>25</v>
@@ -2096,10 +2095,10 @@
         <v>51</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>37</v>
@@ -2111,22 +2110,22 @@
         <v>48</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I25" s="3">
         <v>2000</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="K25" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="L25" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>25</v>
@@ -2138,7 +2137,7 @@
         <v>28</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2146,10 +2145,10 @@
         <v>51</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>20</v>
@@ -2161,16 +2160,16 @@
         <v>38</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I26" s="3">
         <v>1911</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>25</v>
@@ -2196,10 +2195,10 @@
         <v>51</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>20</v>
@@ -2208,31 +2207,31 @@
         <v>31</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I27" s="3">
         <v>2019</v>
       </c>
       <c r="J27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K27" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L27" s="2" t="s">
+      <c r="M27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>28</v>
@@ -2243,10 +2242,10 @@
         <v>51</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>37</v>
@@ -2258,22 +2257,22 @@
         <v>38</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I28" s="3">
         <v>2019</v>
       </c>
       <c r="J28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>25</v>
@@ -2290,13 +2289,13 @@
     </row>
     <row r="30" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>20</v>
@@ -2308,10 +2307,10 @@
         <v>22</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I30" s="3">
         <v>1877</v>
@@ -2337,13 +2336,13 @@
     </row>
     <row r="31" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>37</v>
@@ -2355,16 +2354,16 @@
         <v>48</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I31" s="3">
         <v>1925</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>25</v>
@@ -2384,28 +2383,28 @@
     </row>
     <row r="32" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I32">
         <v>1870</v>
@@ -2431,28 +2430,28 @@
     </row>
     <row r="33" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I33" s="3">
         <v>1884</v>
@@ -2478,34 +2477,34 @@
     </row>
     <row r="34" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>38</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I34" s="3">
         <v>1925</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>25</v>
@@ -2525,34 +2524,34 @@
     </row>
     <row r="35" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>38</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I35" s="3">
         <v>1920</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>25</v>
@@ -2572,13 +2571,13 @@
     </row>
     <row r="36" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>20</v>
@@ -2590,16 +2589,16 @@
         <v>22</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I36" s="3">
         <v>1920</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>25</v>
@@ -2622,13 +2621,13 @@
     </row>
     <row r="37" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>37</v>
@@ -2640,16 +2639,16 @@
         <v>38</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I37" s="3">
         <v>1920</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>25</v>
@@ -2669,13 +2668,13 @@
     </row>
     <row r="38" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>20</v>
@@ -2687,10 +2686,10 @@
         <v>22</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I38" s="2">
         <v>1879</v>
@@ -2728,13 +2727,13 @@
     </row>
     <row r="39" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>20</v>
@@ -2746,22 +2745,22 @@
         <v>22</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I39" s="3">
         <v>1827</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>25</v>
@@ -2776,13 +2775,13 @@
     </row>
     <row r="40" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>37</v>
@@ -2794,16 +2793,16 @@
         <v>22</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I40" s="3">
         <v>1920</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>25</v>
@@ -2815,7 +2814,7 @@
         <v>25</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O40" s="2" t="s">
         <v>28</v>
@@ -2823,40 +2822,40 @@
     </row>
     <row r="41" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I41" s="3">
         <v>2013</v>
       </c>
       <c r="J41" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>25</v>
@@ -2871,46 +2870,46 @@
     </row>
     <row r="42" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I42" s="3">
         <v>2013</v>
       </c>
       <c r="J42" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L42" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="K42" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="M42" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>28</v>
@@ -2918,13 +2917,13 @@
     </row>
     <row r="43" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>20</v>
@@ -2936,16 +2935,16 @@
         <v>22</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I43" s="3">
         <v>2011</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>25</v>
@@ -2957,7 +2956,7 @@
         <v>25</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O43" s="2" t="s">
         <v>28</v>
@@ -2965,13 +2964,13 @@
     </row>
     <row r="44" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>37</v>
@@ -2983,16 +2982,16 @@
         <v>38</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I44" s="3">
         <v>2011</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>25</v>
@@ -3004,7 +3003,7 @@
         <v>25</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>28</v>
@@ -3028,46 +3027,46 @@
     </row>
     <row r="46" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="C46" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>48</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>202</v>
+        <v>191</v>
+      </c>
+      <c r="H46" t="s">
+        <v>200</v>
       </c>
       <c r="I46" s="3">
         <v>1964</v>
       </c>
       <c r="J46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L46" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="K46" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="M46" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>28</v>
@@ -3075,40 +3074,40 @@
     </row>
     <row r="47" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I47" s="3">
         <v>1809</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>25</v>
@@ -3122,34 +3121,34 @@
     </row>
     <row r="48" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>38</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I48" s="3">
         <v>1931</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>25</v>
@@ -3169,34 +3168,34 @@
     </row>
     <row r="49" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I49">
         <v>1931</v>
       </c>
       <c r="J49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K49" t="s">
         <v>25</v>
@@ -3208,7 +3207,7 @@
         <v>25</v>
       </c>
       <c r="N49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>28</v>
@@ -3216,34 +3215,34 @@
     </row>
     <row r="50" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I50" s="3">
         <v>1847</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>25</v>
@@ -3263,13 +3262,13 @@
     </row>
     <row r="51" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>20</v>
@@ -3281,19 +3280,19 @@
         <v>48</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I51" s="3">
         <v>1999</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>34</v>
@@ -3310,13 +3309,13 @@
     </row>
     <row r="52" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>37</v>
@@ -3328,19 +3327,19 @@
         <v>38</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I52" s="3">
         <v>1999</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>34</v>

</xml_diff>